<commit_message>
[mod] updated report and results.
</commit_message>
<xml_diff>
--- a/blur_results.xlsx
+++ b/blur_results.xlsx
@@ -18,12 +18,48 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+  <si>
+    <t>Thread_x</t>
+  </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>Thread_y</t>
+  </si>
+  <si>
+    <t>Block_x</t>
+  </si>
+  <si>
+    <t>Block_y</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,18 +82,408 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8996.341797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5069.11377</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3808.34375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3144.701904</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2785.800049</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2529.459473</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2333.996582</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2182.471191</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2138698392"/>
+        <c:axId val="-2138799592"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2138698392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2138799592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2138799592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2138698392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8996.358398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4500.297852</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3024.558105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2251.532471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1829.491699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1530.890381</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1302.559692</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1126.928955</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2117935960"/>
+        <c:axId val="-2138595080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2117935960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2138595080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2138595080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2117935960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,13 +808,252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>8996.3417969999991</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>8996.3447269999997</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>8996.3583980000003</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>8996.3574219999991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5069.1137699999999</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5069.1210940000001</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4500.2978519999997</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>4500.298828</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3808.34375</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3808.258057</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3024.5581050000001</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>3024.5498050000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3144.701904</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3144.6428219999998</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2251.532471</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>2251.5234380000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2785.8000489999999</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>2785.6906739999999</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1829.4916989999999</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>1829.4819339999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2529.4594729999999</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>2529.4746089999999</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1530.8903809999999</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>1530.8867190000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2333.9965820000002</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>2333.993164</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1302.559692</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>1302.5694579999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2182.4711910000001</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>2182.4360350000002</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1126.9289550000001</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>1126.9174800000001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>